<commit_message>
added conn.close to main.py. added field in writer for abv
</commit_message>
<xml_diff>
--- a/InheritanceProject/data/excel_output/beverage_report.xlsx
+++ b/InheritanceProject/data/excel_output/beverage_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>price</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>alcohol_content</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -462,6 +467,9 @@
       <c r="C2" t="n">
         <v>44.99</v>
       </c>
+      <c r="D2" t="n">
+        <v>13.5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -475,6 +483,9 @@
       <c r="C3" t="n">
         <v>9.99</v>
       </c>
+      <c r="D3" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -488,6 +499,9 @@
       <c r="C4" t="n">
         <v>22.99</v>
       </c>
+      <c r="D4" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -501,6 +515,9 @@
       <c r="C5" t="n">
         <v>13.99</v>
       </c>
+      <c r="D5" t="n">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -514,6 +531,9 @@
       <c r="C6" t="n">
         <v>12.99</v>
       </c>
+      <c r="D6" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -527,6 +547,9 @@
       <c r="C7" t="n">
         <v>10.99</v>
       </c>
+      <c r="D7" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -540,6 +563,9 @@
       <c r="C8" t="n">
         <v>13.99</v>
       </c>
+      <c r="D8" t="n">
+        <v>13.5</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -553,6 +579,9 @@
       <c r="C9" t="n">
         <v>14.99</v>
       </c>
+      <c r="D9" t="n">
+        <v>13.8</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -566,6 +595,9 @@
       <c r="C10" t="n">
         <v>10.99</v>
       </c>
+      <c r="D10" t="n">
+        <v>14.2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -579,6 +611,9 @@
       <c r="C11" t="n">
         <v>9.99</v>
       </c>
+      <c r="D11" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -592,6 +627,9 @@
       <c r="C12" t="n">
         <v>10.99</v>
       </c>
+      <c r="D12" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -605,6 +643,9 @@
       <c r="C13" t="n">
         <v>13.99</v>
       </c>
+      <c r="D13" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -618,6 +659,9 @@
       <c r="C14" t="n">
         <v>12.99</v>
       </c>
+      <c r="D14" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -631,6 +675,9 @@
       <c r="C15" t="n">
         <v>17.99</v>
       </c>
+      <c r="D15" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -644,6 +691,9 @@
       <c r="C16" t="n">
         <v>18.99</v>
       </c>
+      <c r="D16" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -657,6 +707,9 @@
       <c r="C17" t="n">
         <v>14.99</v>
       </c>
+      <c r="D17" t="n">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -670,6 +723,9 @@
       <c r="C18" t="n">
         <v>9.99</v>
       </c>
+      <c r="D18" t="n">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -683,6 +739,7 @@
       <c r="C19" t="n">
         <v>0.99</v>
       </c>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -696,6 +753,7 @@
       <c r="C20" t="n">
         <v>1.79</v>
       </c>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -709,6 +767,7 @@
       <c r="C21" t="n">
         <v>2.49</v>
       </c>
+      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -722,6 +781,7 @@
       <c r="C22" t="n">
         <v>2.99</v>
       </c>
+      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -735,6 +795,7 @@
       <c r="C23" t="n">
         <v>2.49</v>
       </c>
+      <c r="D23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
created xlsx beverage lists of mixed products in place of lists of the same type in excel_input. produced new excel output with same results after modifying query in excel_writer.py
</commit_message>
<xml_diff>
--- a/InheritanceProject/data/excel_output/beverage_report.xlsx
+++ b/InheritanceProject/data/excel_output/beverage_report.xlsx
@@ -474,314 +474,330 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mondavi Chardonnay</t>
+          <t>Russian River Pliny the Elder</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25.36</v>
+        <v>16</v>
       </c>
       <c r="C3" t="n">
-        <v>9.99</v>
+        <v>18.99</v>
       </c>
       <c r="D3" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lange Pinot Noir</t>
+          <t>Iced Tea</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25.36</v>
+        <v>18</v>
       </c>
       <c r="C4" t="n">
-        <v>22.99</v>
-      </c>
-      <c r="D4" t="n">
-        <v>13</v>
+        <v>1.79</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Matua Sauvignon Blanc</t>
+          <t>Les Jamelles Syrah</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>25.36</v>
       </c>
       <c r="C5" t="n">
-        <v>13.99</v>
+        <v>10.99</v>
       </c>
       <c r="D5" t="n">
-        <v>12.5</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Alamos Malbec</t>
+          <t>Goose Island IPA</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25.36</v>
+        <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>12.99</v>
+        <v>9.99</v>
       </c>
       <c r="D6" t="n">
-        <v>14</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Relax Riesling</t>
+          <t>Mondavi Chardonnay</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>25.36</v>
       </c>
       <c r="C7" t="n">
-        <v>10.99</v>
+        <v>9.99</v>
       </c>
       <c r="D7" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>OVZ Zinfandel</t>
+          <t>Old Nation M-43</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>25.36</v>
+        <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>13.99</v>
+        <v>14.99</v>
       </c>
       <c r="D8" t="n">
-        <v>13.5</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Trapiche Malbec</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>25.36</v>
+        <v>16.9</v>
       </c>
       <c r="C9" t="n">
-        <v>14.99</v>
-      </c>
-      <c r="D9" t="n">
-        <v>13.8</v>
+        <v>0.99</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Les Jamelles Syrah</t>
+          <t>Tomaiolo Pinot Grigio</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>25.36</v>
       </c>
       <c r="C10" t="n">
-        <v>10.99</v>
+        <v>9.99</v>
       </c>
       <c r="D10" t="n">
-        <v>14.2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tomaiolo Pinot Grigio</t>
+          <t>Murphys Irish Stout</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>25.36</v>
+        <v>16</v>
       </c>
       <c r="C11" t="n">
-        <v>9.99</v>
+        <v>10.99</v>
       </c>
       <c r="D11" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Murphys Irish Stout</t>
+          <t>Relax Riesling</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>16</v>
+        <v>25.36</v>
       </c>
       <c r="C12" t="n">
         <v>10.99</v>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Weldwerks Juicy Bits</t>
+          <t>Milk</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>13.99</v>
-      </c>
-      <c r="D13" t="n">
-        <v>8</v>
+        <v>2.99</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Smithwicks</t>
+          <t>OVZ Zinfandel</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>16</v>
+        <v>25.36</v>
       </c>
       <c r="C14" t="n">
-        <v>12.99</v>
+        <v>13.99</v>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Alchemist Heady Topper</t>
+          <t>Iced Coffee</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>16</v>
       </c>
       <c r="C15" t="n">
-        <v>17.99</v>
-      </c>
-      <c r="D15" t="n">
-        <v>4.5</v>
+        <v>2.49</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Russian River Pliny the Elder</t>
+          <t>Lange Pinot Noir</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>16</v>
+        <v>25.36</v>
       </c>
       <c r="C16" t="n">
-        <v>18.99</v>
+        <v>22.99</v>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Old Nation M-43</t>
+          <t>Alchemist Heady Topper</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>14.99</v>
+        <v>17.99</v>
       </c>
       <c r="D17" t="n">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Goose Island IPA</t>
+          <t>Smithwicks</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>9.99</v>
+        <v>12.99</v>
       </c>
       <c r="D18" t="n">
-        <v>5.9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Alamos Malbec</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>16.9</v>
+        <v>25.36</v>
       </c>
       <c r="C19" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="D19" t="inlineStr"/>
+        <v>12.99</v>
+      </c>
+      <c r="D19" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Iced Tea</t>
+          <t>Trapiche Malbec</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>18</v>
+        <v>25.36</v>
       </c>
       <c r="C20" t="n">
-        <v>1.79</v>
-      </c>
-      <c r="D20" t="inlineStr"/>
+        <v>14.99</v>
+      </c>
+      <c r="D20" t="n">
+        <v>13.8</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Iced Coffee</t>
+          <t>Weldwerks Juicy Bits</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>16</v>
       </c>
       <c r="C21" t="n">
-        <v>2.49</v>
-      </c>
-      <c r="D21" t="inlineStr"/>
+        <v>13.99</v>
+      </c>
+      <c r="D21" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Milk</t>
+          <t>Matua Sauvignon Blanc</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>32</v>
+        <v>25.36</v>
       </c>
       <c r="C22" t="n">
-        <v>2.99</v>
-      </c>
-      <c r="D22" t="inlineStr"/>
+        <v>13.99</v>
+      </c>
+      <c r="D22" t="n">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -795,7 +811,11 @@
       <c r="C23" t="n">
         <v>2.49</v>
       </c>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>